<commit_message>
Updated the EoS from matter density to energy density
</commit_message>
<xml_diff>
--- a/data_eos/eos_middle.xlsx
+++ b/data_eos/eos_middle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/eos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/data_eos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_F25DC773A252ABDACC10484041DA509C5ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6697F3B-9881-464B-A4A0-DE966B74664C}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC10484041DA509C5ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27444792-3637-4B4C-9A7B-51E430EE9D9C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,10 +94,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,8 +361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -381,7 +377,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.9804822000000001E-18</v>
+        <v>3.9311744250000005E-18</v>
       </c>
       <c r="B2">
         <v>5.6506710149999995E-31</v>
@@ -389,7 +385,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>4.0091703600000008E-18</v>
+        <v>3.9508975350000003E-18</v>
       </c>
       <c r="B3">
         <v>5.6506710150000004E-30</v>
@@ -397,7 +393,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4.135577565E-18</v>
+        <v>4.0764082350000005E-18</v>
       </c>
       <c r="B4">
         <v>5.6506710150000005E-29</v>
@@ -405,7 +401,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5.8882448400000006E-18</v>
+        <v>5.8021803600000001E-18</v>
       </c>
       <c r="B5">
         <v>6.7695092550000006E-28</v>
@@ -413,7 +409,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>8.3392895100000012E-18</v>
+        <v>8.2030207500000005E-18</v>
       </c>
       <c r="B6">
         <v>7.8327641849999998E-27</v>
@@ -421,7 +417,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2.2914667800000003E-17</v>
+        <v>2.25560658E-17</v>
       </c>
       <c r="B7">
         <v>9.5119180500000005E-26</v>
@@ -429,7 +425,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1.069530465E-16</v>
+        <v>1.060565415E-16</v>
       </c>
       <c r="B8">
         <v>3.2561061599999997E-24</v>
@@ -437,7 +433,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5.8371440550000003E-16</v>
+        <v>5.7519760800000005E-16</v>
       </c>
       <c r="B9">
         <v>1.0632549299999999E-22</v>
@@ -445,7 +441,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5.3028270750000007E-15</v>
+        <v>5.2221416250000006E-15</v>
       </c>
       <c r="B10">
         <v>5.4516469050000003E-21</v>
@@ -453,7 +449,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1.3313099250000001E-14</v>
+        <v>1.3115868149999999E-14</v>
       </c>
       <c r="B11">
         <v>2.7791655000000003E-20</v>
@@ -461,7 +457,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3.34575666E-14</v>
+        <v>3.2946558750000004E-14</v>
       </c>
       <c r="B12">
         <v>1.359998085E-19</v>
@@ -469,7 +465,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>8.4029413650000012E-14</v>
+        <v>8.2729481400000003E-14</v>
       </c>
       <c r="B13">
         <v>6.4395954150000001E-19</v>
@@ -477,7 +473,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2.1112692750000002E-13</v>
+        <v>2.0789950950000002E-13</v>
       </c>
       <c r="B14">
         <v>2.94591543E-18</v>
@@ -485,7 +481,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>5.3019305700000001E-13</v>
+        <v>5.2221416250000003E-13</v>
       </c>
       <c r="B15">
         <v>1.297242735E-17</v>
@@ -493,7 +489,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1.3313099250000001E-12</v>
+        <v>1.3115868150000002E-12</v>
       </c>
       <c r="B16">
         <v>5.4579224400000002E-17</v>
@@ -501,7 +497,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3.3457566600000002E-12</v>
+        <v>3.29555238E-12</v>
       </c>
       <c r="B17">
         <v>2.1883687050000003E-16</v>
@@ -509,7 +505,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>4.2117804899999999E-12</v>
+        <v>4.1481286350000001E-12</v>
       </c>
       <c r="B18">
         <v>2.9423294100000003E-16</v>
@@ -517,7 +513,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>8.4029413650000008E-12</v>
+        <v>8.2774306650000005E-12</v>
       </c>
       <c r="B19">
         <v>8.0282022749999996E-16</v>
@@ -525,7 +521,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1.6764643500000001E-11</v>
+        <v>1.65136221E-11</v>
       </c>
       <c r="B20">
         <v>2.1444399600000002E-15</v>
@@ -533,7 +529,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>3.3457566600000004E-11</v>
+        <v>3.2955523800000003E-11</v>
       </c>
       <c r="B21">
         <v>5.62825839E-15</v>
@@ -541,7 +537,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6.6744797250000002E-11</v>
+        <v>6.5776571850000001E-11</v>
       </c>
       <c r="B22">
         <v>1.4568206250000001E-14</v>
@@ -549,7 +545,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>1.3313099250000001E-10</v>
+        <v>1.3124833200000001E-10</v>
       </c>
       <c r="B23">
         <v>3.7348398300000001E-14</v>
@@ -557,7 +553,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>1.67646435E-10</v>
+        <v>1.6522587150000001E-10</v>
       </c>
       <c r="B24">
         <v>4.888641765E-14</v>
@@ -565,7 +561,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>2.6572408200000001E-10</v>
+        <v>2.6195876099999999E-10</v>
       </c>
       <c r="B25">
         <v>9.1174558500000013E-14</v>
@@ -573,7 +569,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>4.2117804899999999E-10</v>
+        <v>4.1517146550000001E-10</v>
       </c>
       <c r="B26">
         <v>1.6943944500000003E-13</v>
@@ -581,7 +577,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>5.3019305699999996E-10</v>
+        <v>5.2266241500000004E-10</v>
       </c>
       <c r="B27">
         <v>2.3102933850000002E-13</v>
@@ -589,7 +585,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>6.6744797250000012E-10</v>
+        <v>6.5821397099999999E-10</v>
       </c>
       <c r="B28">
         <v>2.817715215E-13</v>
@@ -597,7 +593,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>8.4029413650000003E-10</v>
+        <v>8.2881887250000003E-10</v>
       </c>
       <c r="B29">
         <v>3.8379379049999999E-13</v>
@@ -605,7 +601,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>1.331309925E-9</v>
+        <v>1.313379825E-9</v>
       </c>
       <c r="B30">
         <v>7.1164566900000002E-13</v>
@@ -613,7 +609,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>2.1112692750000001E-9</v>
+        <v>2.0825811150000002E-9</v>
       </c>
       <c r="B31">
         <v>1.3178623499999999E-12</v>
@@ -621,7 +617,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>3.3457566600000003E-9</v>
+        <v>3.3018279150000003E-9</v>
       </c>
       <c r="B32">
         <v>2.44028661E-12</v>
@@ -629,7 +625,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>4.2117804900000004E-9</v>
+        <v>4.1570936849999999E-9</v>
       </c>
       <c r="B33">
         <v>3.1673521650000002E-12</v>
@@ -637,7 +633,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>5.30193057E-9</v>
+        <v>5.2320031800000006E-9</v>
       </c>
       <c r="B34">
         <v>4.309499535E-12</v>
@@ -645,7 +641,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>6.6744797250000002E-9</v>
+        <v>6.5920012650000006E-9</v>
       </c>
       <c r="B35">
         <v>5.8631427000000003E-12</v>
@@ -653,7 +649,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>8.4029413650000001E-9</v>
+        <v>8.2980502800000007E-9</v>
       </c>
       <c r="B36">
         <v>7.9726189650000001E-12</v>
@@ -661,7 +657,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>1.0578759000000001E-8</v>
+        <v>1.0453248300000001E-8</v>
       </c>
       <c r="B37">
         <v>1.0838745449999999E-11</v>
@@ -669,7 +665,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>1.3313099250000001E-8</v>
+        <v>1.3160693400000001E-8</v>
       </c>
       <c r="B38">
         <v>1.40034081E-11</v>
@@ -677,7 +673,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>1.6764643500000002E-8</v>
+        <v>1.6567412400000001E-8</v>
       </c>
       <c r="B39">
         <v>1.9041766200000001E-11</v>
@@ -685,7 +681,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>2.1112692750000002E-8</v>
+        <v>2.0870636399999999E-8</v>
       </c>
       <c r="B40">
         <v>2.5891064400000001E-11</v>
@@ -693,7 +689,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>2.6572408200000002E-8</v>
+        <v>2.6276561549999999E-8</v>
       </c>
       <c r="B41">
         <v>3.3287230649999998E-11</v>
@@ -701,7 +697,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>3.3457566599999998E-8</v>
+        <v>3.3098964600000003E-8</v>
       </c>
       <c r="B42">
         <v>4.5255572399999997E-11</v>
@@ -709,7 +705,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>4.2117804900000006E-8</v>
+        <v>4.1678517449999998E-8</v>
       </c>
       <c r="B43">
         <v>6.1545068250000005E-11</v>
@@ -717,7 +713,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>5.30193057E-8</v>
+        <v>5.2463472600000006E-8</v>
       </c>
       <c r="B44">
         <v>8.3643916500000004E-11</v>
@@ -725,7 +721,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>6.6744797250000012E-8</v>
+        <v>6.6126208800000006E-8</v>
       </c>
       <c r="B45">
         <v>1.137664845E-10</v>
@@ -733,7 +729,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>8.4029413650000001E-8</v>
+        <v>8.3231524200000011E-8</v>
       </c>
       <c r="B46">
         <v>1.4532346050000003E-10</v>
@@ -741,7 +737,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>9.3057219000000011E-8</v>
+        <v>9.2250364500000008E-8</v>
       </c>
       <c r="B47">
         <v>1.6181915250000001E-10</v>
@@ -749,7 +745,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1.0578759E-7</v>
+        <v>1.0480143450000001E-7</v>
       </c>
       <c r="B48">
         <v>1.840524765E-10</v>
@@ -757,7 +753,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>1.331309925E-7</v>
+        <v>1.3205518649999999E-7</v>
       </c>
       <c r="B49">
         <v>2.5021454550000001E-10</v>
@@ -765,7 +761,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>1.6764643500000001E-7</v>
+        <v>1.663016775E-7</v>
       </c>
       <c r="B50">
         <v>3.25431315E-10</v>
@@ -773,7 +769,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>2.1668525850000002E-7</v>
+        <v>2.1498189900000002E-7</v>
       </c>
       <c r="B51">
         <v>4.3668758550000004E-10</v>
@@ -781,7 +777,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>2.2493310450000003E-7</v>
+        <v>2.23050444E-7</v>
       </c>
       <c r="B52">
         <v>4.4143906200000007E-10</v>
@@ -789,7 +785,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>2.6330351850000004E-7</v>
+        <v>2.6151050850000001E-7</v>
       </c>
       <c r="B53">
         <v>4.6725840599999997E-10</v>
@@ -797,7 +793,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>3.3278265599999999E-7</v>
+        <v>3.3063104400000002E-7</v>
       </c>
       <c r="B54">
         <v>5.0903553900000008E-10</v>
@@ -805,7 +801,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>4.0082738550000002E-7</v>
+        <v>3.9831717149999999E-7</v>
       </c>
       <c r="B55">
         <v>5.5000581750000008E-10</v>
@@ -813,7 +809,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>4.895813805000001E-7</v>
+        <v>4.8653326350000004E-7</v>
       </c>
       <c r="B56">
         <v>6.0594772950000001E-10</v>
@@ -821,7 +817,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>6.0164450550000002E-7</v>
+        <v>5.9823778650000006E-7</v>
       </c>
       <c r="B57">
         <v>6.8143345050000003E-10</v>
@@ -829,7 +825,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>7.4006487750000004E-7</v>
+        <v>7.3576165349999998E-7</v>
       </c>
       <c r="B58">
         <v>7.8273851550000011E-10</v>
@@ -837,7 +833,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>8.4235609800000007E-7</v>
+        <v>8.4181819499999997E-7</v>
       </c>
       <c r="B59">
         <v>5.3288257200000009E-10</v>
@@ -845,7 +841,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>3.3690657900000003E-6</v>
+        <v>3.3726518100000002E-6</v>
       </c>
       <c r="B60">
         <v>5.1988324950000004E-9</v>
@@ -853,7 +849,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>6.7390280850000003E-6</v>
+        <v>6.7506826500000008E-6</v>
       </c>
       <c r="B61">
         <v>1.0453248300000001E-8</v>
@@ -861,7 +857,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>1.010361135E-5</v>
+        <v>1.0130506500000002E-5</v>
       </c>
       <c r="B62">
         <v>1.8692129250000002E-8</v>
@@ -869,7 +865,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>1.347447015E-5</v>
+        <v>1.3519295400000001E-5</v>
       </c>
       <c r="B63">
         <v>2.8831600800000001E-8</v>
@@ -877,7 +873,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>1.684532895E-5</v>
+        <v>1.6908084299999999E-5</v>
       </c>
       <c r="B64">
         <v>4.0477200750000006E-8</v>
@@ -885,7 +881,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>2.0216187750000003E-5</v>
+        <v>2.0296873200000001E-5</v>
       </c>
       <c r="B65">
         <v>5.3440663050000008E-8</v>
@@ -893,7 +889,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>2.3587046549999999E-5</v>
+        <v>2.3685662100000004E-5</v>
       </c>
       <c r="B66">
         <v>6.7632337200000001E-8</v>
@@ -901,7 +897,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>2.6957905350000003E-5</v>
+        <v>2.7083416050000002E-5</v>
       </c>
       <c r="B67">
         <v>8.3016363E-8</v>
@@ -909,7 +905,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>3.0319799100000003E-5</v>
+        <v>3.048117E-5</v>
       </c>
       <c r="B68">
         <v>9.9512055000000012E-8</v>
@@ -917,7 +913,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>3.3690657899999999E-5</v>
+        <v>3.3878923950000002E-5</v>
       </c>
       <c r="B69">
         <v>1.1726285400000001E-7</v>
@@ -925,7 +921,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>3.7061516700000003E-5</v>
+        <v>3.7276677900000003E-5</v>
       </c>
       <c r="B70">
         <v>1.3608945899999999E-7</v>
@@ -933,7 +929,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>4.0432375500000006E-5</v>
+        <v>4.0683396900000004E-5</v>
       </c>
       <c r="B71">
         <v>1.5617117100000001E-7</v>
@@ -941,7 +937,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>4.3803234300000002E-5</v>
+        <v>4.4090115899999999E-5</v>
       </c>
       <c r="B72">
         <v>1.7750799000000002E-7</v>
@@ -949,7 +945,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>4.7174093099999999E-5</v>
+        <v>4.74968349E-5</v>
       </c>
       <c r="B73">
         <v>2.0001026550000001E-7</v>
@@ -957,7 +953,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>5.0535986850000002E-5</v>
+        <v>5.0903553900000001E-5</v>
       </c>
       <c r="B74">
         <v>2.2385729850000001E-7</v>
@@ -965,7 +961,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>5.3906845650000006E-5</v>
+        <v>5.4310272900000002E-5</v>
       </c>
       <c r="B75">
         <v>2.489594385E-7</v>
@@ -973,7 +969,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>5.7277704450000002E-5</v>
+        <v>5.7716991899999996E-5</v>
       </c>
       <c r="B76">
         <v>2.7549598650000005E-7</v>
@@ -981,7 +977,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>6.0648563250000005E-5</v>
+        <v>6.1132675950000004E-5</v>
       </c>
       <c r="B77">
         <v>3.0346694250000003E-7</v>
@@ -989,7 +985,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>6.4019422049999995E-5</v>
+        <v>6.4548360000000004E-5</v>
       </c>
       <c r="B78">
         <v>3.3287230650000004E-7</v>
@@ -997,7 +993,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>6.7390280850000012E-5</v>
+        <v>6.7964044050000005E-5</v>
       </c>
       <c r="B79">
         <v>3.6344312699999999E-7</v>
@@ -1005,7 +1001,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>7.8058690350000002E-5</v>
+        <v>7.8802789500000012E-5</v>
       </c>
       <c r="B80">
         <v>4.0073773500000002E-7</v>
@@ -1013,7 +1009,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>9.6015685499999993E-5</v>
+        <v>9.7001841000000002E-5</v>
       </c>
       <c r="B81">
         <v>6.4207688099999995E-7</v>
@@ -1021,7 +1017,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>1.058772405E-4</v>
+        <v>1.0713234750000001E-4</v>
       </c>
       <c r="B82">
         <v>8.1528164700000008E-7</v>
@@ -1029,7 +1025,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>1.1645599950000001E-4</v>
+        <v>1.1789040750000001E-4</v>
       </c>
       <c r="B83">
         <v>1.03456677E-6</v>
@@ -1037,7 +1033,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>1.2775196250000001E-4</v>
+        <v>1.2945532200000001E-4</v>
       </c>
       <c r="B84">
         <v>1.31248332E-6</v>
@@ -1045,7 +1041,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>1.3976512950000003E-4</v>
+        <v>1.4164779E-4</v>
       </c>
       <c r="B85">
         <v>1.659430755E-6</v>
@@ -1053,7 +1049,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>1.4819227650000001E-4</v>
+        <v>1.5043353900000002E-4</v>
       </c>
       <c r="B86">
         <v>1.939140315E-6</v>
@@ -1061,7 +1057,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>1.6172950200000002E-4</v>
+        <v>1.6432936650000003E-4</v>
       </c>
       <c r="B87">
         <v>2.7468913200000002E-6</v>
@@ -1069,7 +1065,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>1.7517707700000001E-4</v>
+        <v>1.7831484450000001E-4</v>
       </c>
       <c r="B88">
         <v>3.7832510999999999E-6</v>
@@ -1077,7 +1073,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>1.8871430250000002E-4</v>
+        <v>1.9238997299999999E-4</v>
       </c>
       <c r="B89">
         <v>5.089458885E-6</v>
@@ -1085,7 +1081,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>2.0216187750000001E-4</v>
+        <v>2.0646510150000002E-4</v>
       </c>
       <c r="B90">
         <v>6.7067539049999999E-6</v>
@@ -1093,7 +1089,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>2.1560945250000002E-4</v>
+        <v>2.2080918150000001E-4</v>
       </c>
       <c r="B91">
         <v>8.681754419999999E-6</v>
@@ -1101,7 +1097,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>2.2914667800000001E-4</v>
+        <v>2.3515326150000003E-4</v>
       </c>
       <c r="B92">
         <v>1.1062871700000001E-5</v>
@@ -1109,7 +1105,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>2.4259425300000002E-4</v>
+        <v>2.4976629300000003E-4</v>
       </c>
       <c r="B93">
         <v>1.390479255E-5</v>
@@ -1117,7 +1113,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>2.5604182800000004E-4</v>
+        <v>2.6446897500000002E-4</v>
       </c>
       <c r="B94">
         <v>1.7257721250000002E-5</v>
@@ -1125,7 +1121,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>2.6957905349999999E-4</v>
+        <v>2.794406085E-4</v>
       </c>
       <c r="B95">
         <v>2.1193378200000002E-5</v>
@@ -1133,7 +1129,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>2.8302662850000001E-4</v>
+        <v>2.9459154300000002E-4</v>
       </c>
       <c r="B96">
         <v>2.5756588650000003E-5</v>
@@ -1141,7 +1137,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>2.9647420350000002E-4</v>
+        <v>3.0992177849999998E-4</v>
       </c>
       <c r="B97">
         <v>3.1028038050000002E-5</v>
@@ -1149,7 +1145,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>3.1001142900000003E-4</v>
+        <v>3.2561061600000003E-4</v>
       </c>
       <c r="B98">
         <v>3.7070481750000002E-5</v>
@@ -1157,7 +1153,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>3.2345900400000005E-4</v>
+        <v>3.4147875450000001E-4</v>
       </c>
       <c r="B99">
         <v>4.3946675100000007E-5</v>
@@ -1165,7 +1161,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>3.3690657900000001E-4</v>
+        <v>3.5770549500000002E-4</v>
       </c>
       <c r="B100">
         <v>5.1746268599999998E-5</v>
@@ -1173,7 +1169,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>3.5044380450000002E-4</v>
+        <v>3.7420118700000002E-4</v>
       </c>
       <c r="B101">
         <v>6.0532017599999999E-5</v>
@@ -1181,7 +1177,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>3.6389137949999998E-4</v>
+        <v>3.9114513150000004E-4</v>
       </c>
       <c r="B102">
         <v>7.0402537650000009E-5</v>
@@ -1189,7 +1185,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>3.7733895449999999E-4</v>
+        <v>4.0844767800000004E-4</v>
       </c>
       <c r="B103">
         <v>8.1420584099999992E-5</v>
@@ -1197,7 +1193,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>3.9087618E-4</v>
+        <v>4.2610882650000002E-4</v>
       </c>
       <c r="B104">
         <v>9.368477250000001E-5</v>
@@ -1205,7 +1201,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>4.0432375500000002E-4</v>
+        <v>4.4430787800000003E-4</v>
       </c>
       <c r="B105">
         <v>1.0722199800000001E-4</v>
@@ -1213,7 +1209,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>4.1777133000000003E-4</v>
+        <v>4.6286553149999996E-4</v>
       </c>
       <c r="B106">
         <v>1.1833866000000001E-4</v>
@@ -1221,7 +1217,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>4.3130855550000004E-4</v>
+        <v>4.8178178700000003E-4</v>
       </c>
       <c r="B107">
         <v>1.30172526E-4</v>
@@ -1229,7 +1225,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>4.4475613050000006E-4</v>
+        <v>5.0114629500000007E-4</v>
       </c>
       <c r="B108">
         <v>1.4281324650000001E-4</v>
@@ -1237,7 +1233,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>4.5820370550000002E-4</v>
+        <v>5.2086940499999998E-4</v>
       </c>
       <c r="B109">
         <v>1.56171171E-4</v>
@@ -1245,7 +1241,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>4.7174093100000008E-4</v>
+        <v>5.4095111699999998E-4</v>
       </c>
       <c r="B110">
         <v>1.7033595E-4</v>
@@ -1253,7 +1249,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>4.8518850600000004E-4</v>
+        <v>5.6148108149999996E-4</v>
       </c>
       <c r="B111">
         <v>1.8539723400000003E-4</v>
@@ -1261,7 +1257,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>4.9863608100000011E-4</v>
+        <v>5.8245929850000012E-4</v>
       </c>
       <c r="B112">
         <v>2.0126537250000001E-4</v>
@@ -1269,7 +1265,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>5.1217330649999996E-4</v>
+        <v>6.0388576800000004E-4</v>
       </c>
       <c r="B113">
         <v>2.1803001599999999E-4</v>
@@ -1277,7 +1273,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>5.2562088150000003E-4</v>
+        <v>6.2576049000000005E-4</v>
       </c>
       <c r="B114">
         <v>2.356911645E-4</v>
@@ -1285,7 +1281,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>5.3906845649999999E-4</v>
+        <v>6.4808346450000002E-4</v>
       </c>
       <c r="B115">
         <v>2.5433846850000003E-4</v>
@@ -1293,7 +1289,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>5.5260568200000005E-4</v>
+        <v>6.7085469149999997E-4</v>
       </c>
       <c r="B116">
         <v>2.7388227750000001E-4</v>
@@ -1301,7 +1297,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>5.6605325700000001E-4</v>
+        <v>6.941638215E-4</v>
       </c>
       <c r="B117">
         <v>2.9441224199999998E-4</v>
@@ -1309,7 +1305,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>5.7950083199999997E-4</v>
+        <v>7.17921204E-4</v>
       </c>
       <c r="B118">
         <v>3.1592836200000001E-4</v>
@@ -1317,7 +1313,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>5.9303805750000004E-4</v>
+        <v>7.4221648949999997E-4</v>
       </c>
       <c r="B119">
         <v>3.3852028800000002E-4</v>
@@ -1325,7 +1321,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>6.064856325E-4</v>
+        <v>7.6704967800000001E-4</v>
       </c>
       <c r="B120">
         <v>3.6209836949999998E-4</v>
@@ -1333,7 +1329,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>6.1993320750000007E-4</v>
+        <v>7.9233111900000003E-4</v>
       </c>
       <c r="B121">
         <v>3.8253868350000001E-4</v>
@@ -1341,7 +1337,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>6.3347043300000002E-4</v>
+        <v>8.1815046300000001E-4</v>
       </c>
       <c r="B122">
         <v>4.0369620150000005E-4</v>
@@ -1349,7 +1345,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>6.4691800800000009E-4</v>
+        <v>8.4432840899999998E-4</v>
       </c>
       <c r="B123">
         <v>4.255709235E-4</v>
@@ -1357,7 +1353,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>6.6036558300000005E-4</v>
+        <v>8.7104425800000002E-4</v>
       </c>
       <c r="B124">
         <v>4.4807319900000002E-4</v>
@@ -1365,7 +1361,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>6.7390280850000012E-4</v>
+        <v>8.9829801000000003E-4</v>
       </c>
       <c r="B125">
         <v>4.7120302800000006E-4</v>
@@ -1373,7 +1369,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>6.8735038350000008E-4</v>
+        <v>9.26089665E-4</v>
       </c>
       <c r="B126">
         <v>4.9513971149999999E-4</v>
@@ -1381,7 +1377,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>7.0079795850000004E-4</v>
+        <v>9.5388132000000009E-4</v>
       </c>
       <c r="B127">
         <v>5.1979359899999994E-4</v>
@@ -1389,7 +1385,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>7.1433518399999999E-4</v>
+        <v>9.8256948000000001E-4</v>
       </c>
       <c r="B128">
         <v>5.4516469050000006E-4</v>
@@ -1397,7 +1393,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>7.2778275899999995E-4</v>
+        <v>1.01125764E-3</v>
       </c>
       <c r="B129">
         <v>5.7125298600000003E-4</v>

</xml_diff>